<commit_message>
fix: rename entity file and add update fields in task spreadsheet
</commit_message>
<xml_diff>
--- a/test_files/csv_test_files/COS10001-Tasks.xlsx
+++ b/test_files/csv_test_files/COS10001-Tasks.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -79,13 +79,16 @@
     <t xml:space="preserve">tutorial_stream</t>
   </si>
   <si>
-    <t xml:space="preserve">has_enabled_numbas_test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">has_numbas_time_delay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">numbas_attempt_limit</t>
+    <t xml:space="preserve">scorm_enabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scorm_time_delay_enabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scorm_attempt_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scorm_allow_review</t>
   </si>
   <si>
     <t xml:space="preserve">New Task Def 1</t>
@@ -183,12 +186,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -381,141 +392,144 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V1" activeCellId="0" sqref="V1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.62109375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="32.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="24.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="22.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="32.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="24.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="22.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="b">
+      <c r="F2" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H2" s="1" t="b">
+      <c r="H2" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="L2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="1" t="n">
         <v>-1</v>
       </c>
-      <c r="N2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="0" t="n">
+      <c r="N2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="P2" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="0" t="n">
+      <c r="P2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="R2" s="0" t="s">
-        <v>28</v>
+      <c r="R2" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>